<commit_message>
Llamar configuracion para llenar emisor en series
</commit_message>
<xml_diff>
--- a/Service.Invoice/wwwroot/layout/excel/Series/SeriesListado.xlsx
+++ b/Service.Invoice/wwwroot/layout/excel/Series/SeriesListado.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Proyectos\API\Service.Invoice\wwwroot\layout\excel\Series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9890C1B8-66DA-493A-9D92-36450F6A6FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7FDC5B-5B9F-4860-B523-0606F53D3B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CostosToma" sheetId="1" r:id="rId1"/>
+    <sheet name="Series" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Series">CostosToma!$A$4:$G$5</definedName>
+    <definedName name="Series">Series!$A$4:$G$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -102,13 +102,13 @@
     <t>{{item.Descripcion}}</t>
   </si>
   <si>
-    <t>{{item.CFDI}}</t>
-  </si>
-  <si>
-    <t>{{item.FechaCreo.Year}}</t>
-  </si>
-  <si>
-    <t>{{item.Activo}}</t>
+    <t>{{item.Año}}</t>
+  </si>
+  <si>
+    <t>{{item.Activo ? "VIGENTE" : "CADUCO"}}</t>
+  </si>
+  <si>
+    <t>{{item.CFDI ? "SI" : "NO"}}</t>
   </si>
 </sst>
 </file>
@@ -208,28 +208,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -612,22 +591,22 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -639,7 +618,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -663,7 +642,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -677,16 +656,16 @@
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
     </row>
   </sheetData>
@@ -694,12 +673,12 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:G4">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>